<commit_message>
Updated unit taxonomy work
</commit_message>
<xml_diff>
--- a/unitTests/source/xodel/unitRelations.xlsx
+++ b/unitTests/source/xodel/unitRelations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Documents/GitHub/xule/unitTests/source/xodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F5FE7A7-8F7F-9F4B-B123-AF219A484002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E348FF-0CC6-0B4B-9F3B-28CFC1D98217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{D8315888-3CE1-6243-B2A8-C1166F657B4C}"/>
+    <workbookView xWindow="3500" yWindow="1700" windowWidth="27640" windowHeight="16940" xr2:uid="{D8315888-3CE1-6243-B2A8-C1166F657B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,115 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="28">
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>sqft</t>
+  </si>
+  <si>
+    <t>sqmi</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>sqyd</t>
+  </si>
+  <si>
+    <t>yd</t>
+  </si>
+  <si>
+    <t>Boe</t>
+  </si>
+  <si>
+    <t>MBoe</t>
+  </si>
+  <si>
+    <t>nstarget</t>
+  </si>
+  <si>
+    <t>utr</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>kilo</t>
+  </si>
+  <si>
+    <t>MMBoe</t>
+  </si>
+  <si>
+    <t>nsSource</t>
+  </si>
+  <si>
+    <t>mega</t>
+  </si>
+  <si>
+    <t>http://www.xbrl.org/2023/arcrole/unit-squared</t>
+  </si>
+  <si>
+    <t>http://www.xbrl.org/2023/arcrole/unit-multiplied</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>nmi</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>dm</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>http://www.xbrl.org/2023/arcrole/converted-convertee</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +166,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,12 +489,373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013ED81D-0876-FA4F-A294-6F37A8E5F936}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D9:D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="49.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>1609.3440000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>0.91439999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{2DEAE640-A4F7-274B-A85F-8213374A729B}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{39E835F7-94BF-EF44-8900-C6861329EFA5}"/>
+    <hyperlink ref="D3:D4" r:id="rId3" display="http://www.xbrl.org/2023/arcrole/unit-squared" xr:uid="{73F1BA5E-E860-C348-8F46-6133AC94EBD8}"/>
+    <hyperlink ref="D6:D7" r:id="rId4" display="http://www.xbrl.org/2023/arcrole/unit-multiplied" xr:uid="{BF5BD8D3-16E3-874B-9007-FB314BFD6705}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{6893E687-6BEF-474D-BEF9-D46B2694E477}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{40F556B8-A273-6240-AE31-AB88CB04FEF3}"/>
+    <hyperlink ref="D11:D15" r:id="rId7" display="http://www.xbrl.org/2023/arcrole/converted-convertee" xr:uid="{A612DDA1-092B-024E-94D2-A1D2EF66ACA0}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{0217D799-27DA-7F41-B8FB-10E6D5F6DCDD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>